<commit_message>
1. Initialised spreadsheets from cmip5 documents based upon cmip5 publication config.
</commit_message>
<xml_diff>
--- a/cmip6/models/mpi-esm1-2-lr/cmip6_mpi-m_mpi-esm1-2-lr_seaice.xlsx
+++ b/cmip6/models/mpi-esm1-2-lr/cmip6_mpi-m_mpi-esm1-2-lr_seaice.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="539">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -154,6 +154,9 @@
     <t>cmip6.seaice.key_properties.name</t>
   </si>
   <si>
+    <t>MPIOM SeaIceComponent</t>
+  </si>
+  <si>
     <t>1.1.1.2 *</t>
   </si>
   <si>
@@ -184,6 +187,10 @@
     <t>NOTE: Double click to expand if text is too long for cell</t>
   </si>
   <si>
+    <t>Sea ice component is included in MPI-OM,_x000D_
+It includes an embedded dynamic/ thermodynamic sea ice model with a viscous- plastic rheology following Hibler (1979)</t>
+  </si>
+  <si>
     <t>1.2.1</t>
   </si>
   <si>
@@ -206,6 +213,9 @@
   </si>
   <si>
     <t>cmip6.seaice.key_properties.variables.prognostic</t>
+  </si>
+  <si>
+    <t>Other: velocity, thickness, sea ice concentration, snow depth</t>
   </si>
   <si>
     <t>Sea ice temperature</t>
@@ -1005,15 +1015,15 @@
     <t>cmip6.seaice.dynamics.rheology</t>
   </si>
   <si>
+    <t>Visco-plastic</t>
+  </si>
+  <si>
     <t>Free-drift</t>
   </si>
   <si>
     <t>Mohr-Coloumb</t>
   </si>
   <si>
-    <t>Visco-plastic</t>
-  </si>
-  <si>
     <t>Elastic-visco-plastic</t>
   </si>
   <si>
@@ -1050,6 +1060,9 @@
     <t>cmip6.seaice.thermodynamics.overview</t>
   </si>
   <si>
+    <t>Dynamic/ thermodynamic sea ice model with a viscous- plastic rheology following Hibler (1979)</t>
+  </si>
+  <si>
     <t>4.2.1</t>
   </si>
   <si>
@@ -1132,6 +1145,9 @@
   </si>
   <si>
     <t>cmip6.seaice.thermodynamics.energy.basal_heat_flux</t>
+  </si>
+  <si>
+    <t>Other: parametrized (calculated in ocean)</t>
   </si>
   <si>
     <t>Heat Reservoir</t>
@@ -1202,6 +1218,9 @@
     <t>cmip6.seaice.thermodynamics.mass.new_ice_formation</t>
   </si>
   <si>
+    <t>Heat budget, minimum ice thickness prescibed</t>
+  </si>
+  <si>
     <t>4.3.1.2 *</t>
   </si>
   <si>
@@ -1458,6 +1477,9 @@
     <t>cmip6.seaice.thermodynamics.melt_ponds.formulation</t>
   </si>
   <si>
+    <t>Other: yes</t>
+  </si>
+  <si>
     <t>Flocco and Feltham (2010)</t>
   </si>
   <si>
@@ -1603,6 +1625,9 @@
   </si>
   <si>
     <t>cmip6.seaice.radiative_processes.surface_albedo</t>
+  </si>
+  <si>
+    <t>Other: seperate for snow cover and sea ice, temperature dependent</t>
   </si>
   <si>
     <t>Delta-Eddington</t>
@@ -2393,14 +2418,16 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -2408,15 +2435,15 @@
         <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
@@ -2424,10 +2451,10 @@
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -2435,50 +2462,52 @@
         <v>41</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="19" spans="1:38" ht="24" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:38" ht="24" customHeight="1">
       <c r="B20" s="13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:38" ht="24" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:38" ht="24" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:38" ht="24" customHeight="1">
@@ -2487,105 +2516,107 @@
       </c>
     </row>
     <row r="25" spans="1:38" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="AA25" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AD25" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AE25" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AF25" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AG25" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AH25" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AI25" s="6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AJ25" s="6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AK25" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AL25" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:38" ht="24" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:38" ht="24" customHeight="1">
       <c r="B29" s="13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:38" ht="24" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:38" ht="24" customHeight="1">
       <c r="A32" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="24" customHeight="1">
       <c r="B33" s="11"/>
       <c r="AA33" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AB33" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AC33" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="24" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="24" customHeight="1">
       <c r="A36" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="24" customHeight="1">
@@ -2593,20 +2624,20 @@
     </row>
     <row r="40" spans="1:29" ht="24" customHeight="1">
       <c r="A40" s="12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="24" customHeight="1">
       <c r="B41" s="13" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="24" customHeight="1">
       <c r="A43" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>40</v>
@@ -2617,10 +2648,10 @@
         <v>41</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="24" customHeight="1">
@@ -2628,10 +2659,10 @@
     </row>
     <row r="47" spans="1:29" ht="24" customHeight="1">
       <c r="A47" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="24" customHeight="1">
@@ -2639,10 +2670,10 @@
         <v>41</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="24" customHeight="1">
@@ -2650,21 +2681,21 @@
     </row>
     <row r="51" spans="1:3" ht="24" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="24" customHeight="1">
       <c r="A52" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="24" customHeight="1">
@@ -2672,23 +2703,23 @@
     </row>
     <row r="56" spans="1:3" ht="24" customHeight="1">
       <c r="A56" s="12" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="24" customHeight="1">
       <c r="B57" s="13" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="24" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="24" customHeight="1">
@@ -2696,15 +2727,15 @@
         <v>41</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="24" customHeight="1">
       <c r="B61" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="178" customHeight="1">
@@ -2712,10 +2743,10 @@
     </row>
     <row r="64" spans="1:3" ht="24" customHeight="1">
       <c r="A64" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="24" customHeight="1">
@@ -2723,10 +2754,10 @@
         <v>41</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="24" customHeight="1">
@@ -2734,10 +2765,10 @@
     </row>
     <row r="68" spans="1:3" ht="24" customHeight="1">
       <c r="A68" s="9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="24" customHeight="1">
@@ -2745,15 +2776,15 @@
         <v>41</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="24" customHeight="1">
       <c r="B70" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="24" customHeight="1">
@@ -2761,10 +2792,10 @@
     </row>
     <row r="73" spans="1:3" ht="24" customHeight="1">
       <c r="A73" s="9" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="24" customHeight="1">
@@ -2772,15 +2803,15 @@
         <v>41</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="24" customHeight="1">
       <c r="B75" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="24" customHeight="1">
@@ -2788,10 +2819,10 @@
     </row>
     <row r="78" spans="1:3" ht="24" customHeight="1">
       <c r="A78" s="9" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="24" customHeight="1">
@@ -2799,15 +2830,15 @@
         <v>41</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="24" customHeight="1">
       <c r="B80" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="24" customHeight="1">
@@ -2815,34 +2846,34 @@
     </row>
     <row r="84" spans="1:3" ht="24" customHeight="1">
       <c r="A84" s="12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="24" customHeight="1">
       <c r="B85" s="13" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="24" customHeight="1">
       <c r="A87" s="9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="24" customHeight="1">
       <c r="A88" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="24" customHeight="1">
@@ -2850,21 +2881,21 @@
     </row>
     <row r="91" spans="1:3" ht="24" customHeight="1">
       <c r="A91" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="24" customHeight="1">
       <c r="A92" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
@@ -2872,21 +2903,21 @@
     </row>
     <row r="95" spans="1:3" ht="24" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="24" customHeight="1">
       <c r="A96" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="24" customHeight="1">
@@ -2894,10 +2925,10 @@
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
       <c r="A99" s="9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1">
@@ -2905,15 +2936,15 @@
         <v>41</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
       <c r="B101" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1">
@@ -2921,23 +2952,23 @@
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
       <c r="A105" s="12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="24" customHeight="1">
       <c r="B106" s="13" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="24" customHeight="1">
       <c r="A108" s="9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="24" customHeight="1">
@@ -2945,15 +2976,15 @@
         <v>41</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1">
       <c r="B110" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="178" customHeight="1">
@@ -2961,10 +2992,10 @@
     </row>
     <row r="113" spans="1:3" ht="24" customHeight="1">
       <c r="A113" s="9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="24" customHeight="1">
@@ -2972,15 +3003,15 @@
         <v>41</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="24" customHeight="1">
       <c r="B115" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="24" customHeight="1">
@@ -2988,10 +3019,10 @@
     </row>
     <row r="118" spans="1:3" ht="24" customHeight="1">
       <c r="A118" s="9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="24" customHeight="1">
@@ -2999,15 +3030,15 @@
         <v>41</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="24" customHeight="1">
       <c r="B120" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1">
@@ -3015,23 +3046,23 @@
     </row>
     <row r="124" spans="1:3" ht="24" customHeight="1">
       <c r="A124" s="12" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="24" customHeight="1">
       <c r="B125" s="13" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="24" customHeight="1">
       <c r="A127" s="9" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="24" customHeight="1">
@@ -3039,15 +3070,15 @@
         <v>41</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="129" spans="1:30" ht="24" customHeight="1">
       <c r="B129" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="130" spans="1:30" ht="178" customHeight="1">
@@ -3055,21 +3086,21 @@
     </row>
     <row r="132" spans="1:30" ht="24" customHeight="1">
       <c r="A132" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="133" spans="1:30" ht="24" customHeight="1">
       <c r="A133" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="134" spans="1:30" ht="24" customHeight="1">
@@ -3080,24 +3111,24 @@
     <row r="135" spans="1:30" ht="24" customHeight="1">
       <c r="B135" s="11"/>
       <c r="AA135" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AB135" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="AC135" s="6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="AD135" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="137" spans="1:30" ht="24" customHeight="1">
       <c r="A137" s="9" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="138" spans="1:30" ht="24" customHeight="1">
@@ -3105,15 +3136,15 @@
         <v>41</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="139" spans="1:30" ht="24" customHeight="1">
       <c r="B139" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="140" spans="1:30" ht="24" customHeight="1">
@@ -3121,21 +3152,21 @@
     </row>
     <row r="142" spans="1:30" ht="24" customHeight="1">
       <c r="A142" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="143" spans="1:30" ht="24" customHeight="1">
       <c r="A143" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="144" spans="1:30" ht="24" customHeight="1">
@@ -3143,10 +3174,10 @@
     </row>
     <row r="146" spans="1:3" ht="24" customHeight="1">
       <c r="A146" s="9" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="24" customHeight="1">
@@ -3154,15 +3185,15 @@
         <v>41</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="24" customHeight="1">
       <c r="B148" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1">
@@ -3222,20 +3253,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>40</v>
@@ -3246,10 +3277,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -3257,10 +3288,10 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -3268,15 +3299,15 @@
         <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
@@ -3284,136 +3315,138 @@
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>203</v>
+      </c>
       <c r="AA19" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="AB19" s="6" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AD19" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
       <c r="B23" s="11"/>
       <c r="AA23" s="6" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AB23" s="6" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="AC23" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AD23" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="24" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="24" customHeight="1">
       <c r="B27" s="11"/>
       <c r="AA27" s="6" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="AB27" s="6" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="AC27" s="6" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="AD27" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="24" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:30" ht="24" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
@@ -3421,21 +3454,21 @@
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
       <c r="A34" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
@@ -3443,10 +3476,10 @@
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
@@ -3454,15 +3487,15 @@
         <v>41</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
       <c r="B39" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="178" customHeight="1">
@@ -3470,34 +3503,34 @@
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
       <c r="A43" s="12" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1">
       <c r="B44" s="13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="24" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1">
       <c r="A47" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
@@ -3508,35 +3541,35 @@
     <row r="49" spans="1:30" ht="24" customHeight="1">
       <c r="B49" s="11"/>
       <c r="AA49" s="6" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="AB49" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="AC49" s="6" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="AD49" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:30" ht="24" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:30" ht="24" customHeight="1">
       <c r="A52" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="24" customHeight="1">
@@ -3544,10 +3577,10 @@
     </row>
     <row r="55" spans="1:30" ht="24" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:30" ht="24" customHeight="1">
@@ -3555,15 +3588,15 @@
         <v>41</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="57" spans="1:30" ht="24" customHeight="1">
       <c r="B57" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:30" ht="178" customHeight="1">
@@ -3571,34 +3604,34 @@
     </row>
     <row r="61" spans="1:30" ht="24" customHeight="1">
       <c r="A61" s="12" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:30" ht="24" customHeight="1">
       <c r="B62" s="13" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:30" ht="24" customHeight="1">
       <c r="A64" s="9" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="24" customHeight="1">
       <c r="A65" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="24" customHeight="1">
@@ -3606,21 +3639,21 @@
     </row>
     <row r="68" spans="1:3" ht="24" customHeight="1">
       <c r="A68" s="9" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="24" customHeight="1">
       <c r="A69" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="24" customHeight="1">
@@ -3628,10 +3661,10 @@
     </row>
     <row r="72" spans="1:3" ht="24" customHeight="1">
       <c r="A72" s="9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="24" customHeight="1">
@@ -3639,15 +3672,15 @@
         <v>41</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="24" customHeight="1">
       <c r="B74" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="24" customHeight="1">
@@ -3655,10 +3688,10 @@
     </row>
     <row r="77" spans="1:3" ht="24" customHeight="1">
       <c r="A77" s="9" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="24" customHeight="1">
@@ -3666,15 +3699,15 @@
         <v>41</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="24" customHeight="1">
       <c r="B79" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="178" customHeight="1">
@@ -3682,10 +3715,10 @@
     </row>
     <row r="82" spans="1:3" ht="24" customHeight="1">
       <c r="A82" s="9" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="24" customHeight="1">
@@ -3693,15 +3726,15 @@
         <v>41</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="24" customHeight="1">
       <c r="B84" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="178" customHeight="1">
@@ -3709,34 +3742,34 @@
     </row>
     <row r="88" spans="1:3" ht="24" customHeight="1">
       <c r="A88" s="12" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="24" customHeight="1">
       <c r="B89" s="13" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="24" customHeight="1">
       <c r="A91" s="9" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="24" customHeight="1">
       <c r="A92" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
@@ -3744,21 +3777,21 @@
     </row>
     <row r="95" spans="1:3" ht="24" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="24" customHeight="1">
       <c r="A96" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="24" customHeight="1">
@@ -3766,10 +3799,10 @@
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
       <c r="A99" s="9" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1">
@@ -3777,15 +3810,15 @@
         <v>41</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
       <c r="B101" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="178" customHeight="1">
@@ -3793,10 +3826,10 @@
     </row>
     <row r="104" spans="1:3" ht="24" customHeight="1">
       <c r="A104" s="9" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
@@ -3804,15 +3837,15 @@
         <v>41</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="24" customHeight="1">
       <c r="B106" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="178" customHeight="1">
@@ -3874,20 +3907,20 @@
   <sheetData>
     <row r="1" spans="1:30" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>40</v>
@@ -3898,10 +3931,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="24" customHeight="1">
@@ -3909,10 +3942,10 @@
     </row>
     <row r="8" spans="1:30" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="24" customHeight="1">
@@ -3920,15 +3953,15 @@
         <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="178" customHeight="1">
@@ -3936,120 +3969,122 @@
     </row>
     <row r="13" spans="1:30" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="24" customHeight="1">
       <c r="B15" s="11"/>
       <c r="AA15" s="6" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="AB15" s="6" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="AC15" s="6" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="AD15" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" ht="24" customHeight="1">
+      <c r="B19" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="19" spans="1:33" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
       <c r="AA19" s="6" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="AB19" s="6" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="AD19" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:33" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:33" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="24" customHeight="1">
       <c r="B23" s="11"/>
       <c r="AA23" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="AB23" s="6" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="AC23" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:33" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:33" ht="24" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:33" ht="24" customHeight="1">
@@ -4060,56 +4095,58 @@
     <row r="28" spans="1:33" ht="24" customHeight="1">
       <c r="B28" s="11"/>
       <c r="AA28" s="6" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AB28" s="6" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="AC28" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:33" ht="24" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:33" ht="24" customHeight="1">
       <c r="A31" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:33" ht="24" customHeight="1">
-      <c r="B32" s="11"/>
+      <c r="B32" s="11" t="s">
+        <v>326</v>
+      </c>
       <c r="AA32" s="6" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="AB32" s="6" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="AC32" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AD32" s="6" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="AE32" s="6" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="AF32" s="6" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="AG32" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -4150,20 +4187,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>40</v>
@@ -4174,10 +4211,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -4185,10 +4222,10 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -4196,186 +4233,190 @@
         <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="24" customHeight="1">
       <c r="B19" s="11"/>
       <c r="AA19" s="6" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="AB19" s="6" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="AD19" s="6" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="AE19" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="24" customHeight="1">
       <c r="B23" s="11"/>
       <c r="AA23" s="6" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="AB23" s="6" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="AC23" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="24" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:31" ht="24" customHeight="1">
       <c r="B27" s="11"/>
       <c r="AA27" s="6" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="AB27" s="6" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="AC27" s="6" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="AD27" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:31" ht="24" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="24" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:31" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
+      <c r="B31" s="11" t="s">
+        <v>370</v>
+      </c>
       <c r="AA31" s="6" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="AB31" s="6" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="AC31" s="6" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="AD31" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
       <c r="A34" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
@@ -4383,10 +4424,10 @@
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
@@ -4394,15 +4435,15 @@
         <v>41</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
       <c r="B39" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="178" customHeight="1">
@@ -4410,10 +4451,10 @@
     </row>
     <row r="42" spans="1:3" ht="24" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
@@ -4421,15 +4462,15 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1">
       <c r="B44" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="178" customHeight="1">
@@ -4437,23 +4478,23 @@
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
       <c r="A48" s="12" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="24" customHeight="1">
       <c r="B49" s="13" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="24" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="24" customHeight="1">
@@ -4461,26 +4502,28 @@
         <v>41</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="24" customHeight="1">
       <c r="B53" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="178" customHeight="1">
-      <c r="B54" s="11"/>
+      <c r="B54" s="11" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="56" spans="1:29" ht="24" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="24" customHeight="1">
@@ -4488,15 +4531,15 @@
         <v>41</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
     </row>
     <row r="58" spans="1:29" ht="24" customHeight="1">
       <c r="B58" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:29" ht="178" customHeight="1">
@@ -4504,41 +4547,41 @@
     </row>
     <row r="61" spans="1:29" ht="24" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
     </row>
     <row r="62" spans="1:29" ht="24" customHeight="1">
       <c r="A62" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
     </row>
     <row r="63" spans="1:29" ht="24" customHeight="1">
       <c r="B63" s="11"/>
       <c r="AA63" s="6" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="AB63" s="6" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="AC63" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="24" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="24" customHeight="1">
@@ -4546,15 +4589,15 @@
         <v>41</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="24" customHeight="1">
       <c r="B67" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="178" customHeight="1">
@@ -4562,10 +4605,10 @@
     </row>
     <row r="70" spans="1:3" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="24" customHeight="1">
@@ -4573,15 +4616,15 @@
         <v>41</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="24" customHeight="1">
       <c r="B72" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="178" customHeight="1">
@@ -4589,34 +4632,34 @@
     </row>
     <row r="76" spans="1:3" ht="24" customHeight="1">
       <c r="A76" s="12" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="24" customHeight="1">
       <c r="B77" s="13" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="24" customHeight="1">
       <c r="A79" s="9" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="24" customHeight="1">
       <c r="A80" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
     </row>
     <row r="81" spans="1:30" ht="24" customHeight="1">
@@ -4624,21 +4667,21 @@
     </row>
     <row r="83" spans="1:30" ht="24" customHeight="1">
       <c r="A83" s="9" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="84" spans="1:30" ht="24" customHeight="1">
       <c r="A84" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
     </row>
     <row r="85" spans="1:30" ht="24" customHeight="1">
@@ -4646,68 +4689,68 @@
     </row>
     <row r="88" spans="1:30" ht="24" customHeight="1">
       <c r="A88" s="12" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
     </row>
     <row r="89" spans="1:30" ht="24" customHeight="1">
       <c r="B89" s="13" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="91" spans="1:30" ht="24" customHeight="1">
       <c r="A91" s="9" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
     </row>
     <row r="92" spans="1:30" ht="24" customHeight="1">
       <c r="A92" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
     </row>
     <row r="93" spans="1:30" ht="24" customHeight="1">
       <c r="B93" s="11"/>
       <c r="AA93" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AB93" s="6" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="AC93" s="6" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="AD93" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="95" spans="1:30" ht="24" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
     </row>
     <row r="96" spans="1:30" ht="24" customHeight="1">
       <c r="A96" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
     <row r="97" spans="1:30" ht="24" customHeight="1">
@@ -4715,10 +4758,10 @@
     </row>
     <row r="99" spans="1:30" ht="24" customHeight="1">
       <c r="A99" s="9" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="100" spans="1:30" ht="24" customHeight="1">
@@ -4726,15 +4769,15 @@
         <v>41</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
     </row>
     <row r="101" spans="1:30" ht="24" customHeight="1">
       <c r="B101" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:30" ht="178" customHeight="1">
@@ -4742,68 +4785,68 @@
     </row>
     <row r="105" spans="1:30" ht="24" customHeight="1">
       <c r="A105" s="12" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
     </row>
     <row r="106" spans="1:30" ht="24" customHeight="1">
       <c r="B106" s="13" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
     </row>
     <row r="108" spans="1:30" ht="24" customHeight="1">
       <c r="A108" s="9" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
     </row>
     <row r="109" spans="1:30" ht="24" customHeight="1">
       <c r="A109" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="110" spans="1:30" ht="24" customHeight="1">
       <c r="B110" s="11"/>
       <c r="AA110" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AB110" s="6" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="AC110" s="6" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="AD110" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="112" spans="1:30" ht="24" customHeight="1">
       <c r="A112" s="9" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
     </row>
     <row r="113" spans="1:29" ht="24" customHeight="1">
       <c r="A113" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="114" spans="1:29" ht="24" customHeight="1">
@@ -4811,10 +4854,10 @@
     </row>
     <row r="116" spans="1:29" ht="24" customHeight="1">
       <c r="A116" s="9" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="117" spans="1:29" ht="24" customHeight="1">
@@ -4822,15 +4865,15 @@
         <v>41</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
     </row>
     <row r="118" spans="1:29" ht="24" customHeight="1">
       <c r="B118" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:29" ht="178" customHeight="1">
@@ -4838,98 +4881,98 @@
     </row>
     <row r="122" spans="1:29" ht="24" customHeight="1">
       <c r="A122" s="12" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
     </row>
     <row r="123" spans="1:29" ht="24" customHeight="1">
       <c r="B123" s="13" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
     </row>
     <row r="125" spans="1:29" ht="24" customHeight="1">
       <c r="A125" s="9" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
     </row>
     <row r="126" spans="1:29" ht="24" customHeight="1">
       <c r="A126" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="C126" s="10" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
     </row>
     <row r="127" spans="1:29" ht="24" customHeight="1">
       <c r="B127" s="11"/>
       <c r="AA127" s="6" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="AB127" s="6" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="AC127" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="1:29" ht="24" customHeight="1">
       <c r="A130" s="12" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
     </row>
     <row r="131" spans="1:29" ht="24" customHeight="1">
       <c r="B131" s="13" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
     </row>
     <row r="133" spans="1:29" ht="24" customHeight="1">
       <c r="A133" s="9" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
     </row>
     <row r="134" spans="1:29" ht="24" customHeight="1">
       <c r="A134" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
     </row>
     <row r="135" spans="1:29" ht="24" customHeight="1">
       <c r="B135" s="11"/>
       <c r="AA135" s="6" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="AB135" s="6" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="AC135" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="137" spans="1:29" ht="24" customHeight="1">
       <c r="A137" s="9" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="138" spans="1:29" ht="24" customHeight="1">
@@ -4937,15 +4980,15 @@
         <v>41</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
     </row>
     <row r="139" spans="1:29" ht="24" customHeight="1">
       <c r="B139" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="140" spans="1:29" ht="178" customHeight="1">
@@ -4953,34 +4996,34 @@
     </row>
     <row r="143" spans="1:29" ht="24" customHeight="1">
       <c r="A143" s="12" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
     </row>
     <row r="144" spans="1:29" ht="24" customHeight="1">
       <c r="B144" s="13" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
     </row>
     <row r="146" spans="1:30" ht="24" customHeight="1">
       <c r="A146" s="9" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
     </row>
     <row r="147" spans="1:30" ht="24" customHeight="1">
       <c r="A147" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
     </row>
     <row r="148" spans="1:30" ht="24" customHeight="1">
@@ -4988,52 +5031,54 @@
     </row>
     <row r="150" spans="1:30" ht="24" customHeight="1">
       <c r="A150" s="9" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
     </row>
     <row r="151" spans="1:30" ht="24" customHeight="1">
       <c r="A151" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
     </row>
     <row r="152" spans="1:30" ht="24" customHeight="1">
-      <c r="B152" s="11"/>
+      <c r="B152" s="11" t="s">
+        <v>479</v>
+      </c>
       <c r="AA152" s="6" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="AB152" s="6" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="AC152" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="154" spans="1:30" ht="24" customHeight="1">
       <c r="A154" s="9" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
     </row>
     <row r="155" spans="1:30" ht="24" customHeight="1">
       <c r="A155" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
     </row>
     <row r="156" spans="1:30" ht="24" customHeight="1">
@@ -5044,48 +5089,48 @@
     <row r="157" spans="1:30" ht="24" customHeight="1">
       <c r="B157" s="11"/>
       <c r="AA157" s="6" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="AB157" s="6" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="AC157" s="6" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="AD157" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="160" spans="1:30" ht="24" customHeight="1">
       <c r="A160" s="12" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="24" customHeight="1">
       <c r="B161" s="13" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="24" customHeight="1">
       <c r="A163" s="9" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="24" customHeight="1">
       <c r="A164" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="24" customHeight="1">
@@ -5093,10 +5138,10 @@
     </row>
     <row r="167" spans="1:3" ht="24" customHeight="1">
       <c r="A167" s="9" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1">
@@ -5104,15 +5149,15 @@
         <v>41</v>
       </c>
       <c r="B168" s="10" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="24" customHeight="1">
       <c r="B169" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="178" customHeight="1">
@@ -5120,21 +5165,21 @@
     </row>
     <row r="172" spans="1:3" ht="24" customHeight="1">
       <c r="A172" s="9" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1">
       <c r="A173" s="14" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="24" customHeight="1">
@@ -5142,10 +5187,10 @@
     </row>
     <row r="176" spans="1:3" ht="24" customHeight="1">
       <c r="A176" s="9" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
     </row>
     <row r="177" spans="1:29" ht="24" customHeight="1">
@@ -5153,15 +5198,15 @@
         <v>41</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
     </row>
     <row r="178" spans="1:29" ht="24" customHeight="1">
       <c r="B178" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="179" spans="1:29" ht="178" customHeight="1">
@@ -5169,10 +5214,10 @@
     </row>
     <row r="181" spans="1:29" ht="24" customHeight="1">
       <c r="A181" s="9" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="182" spans="1:29" ht="24" customHeight="1">
@@ -5180,10 +5225,10 @@
         <v>41</v>
       </c>
       <c r="B182" s="10" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
     </row>
     <row r="183" spans="1:29" ht="24" customHeight="1">
@@ -5191,33 +5236,33 @@
     </row>
     <row r="185" spans="1:29" ht="24" customHeight="1">
       <c r="A185" s="9" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="186" spans="1:29" ht="24" customHeight="1">
       <c r="A186" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
     </row>
     <row r="187" spans="1:29" ht="24" customHeight="1">
       <c r="B187" s="11"/>
       <c r="AA187" s="6" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="AB187" s="6" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="AC187" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -5306,20 +5351,20 @@
   <sheetData>
     <row r="1" spans="1:30" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>40</v>
@@ -5330,10 +5375,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="24" customHeight="1">
@@ -5341,10 +5386,10 @@
     </row>
     <row r="8" spans="1:30" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="24" customHeight="1">
@@ -5352,15 +5397,15 @@
         <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="24" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="178" customHeight="1">
@@ -5368,55 +5413,57 @@
     </row>
     <row r="13" spans="1:30" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="24" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="24" customHeight="1">
-      <c r="B15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>529</v>
+      </c>
       <c r="AA15" s="6" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="AB15" s="6" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="AC15" s="6" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="AD15" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
@@ -5427,16 +5474,16 @@
     <row r="20" spans="1:30" ht="24" customHeight="1">
       <c r="B20" s="11"/>
       <c r="AA20" s="6" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="AB20" s="6" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="AC20" s="6" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
       <c r="AD20" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>